<commit_message>
Correções RNF e RF 01.10.24
</commit_message>
<xml_diff>
--- a/CCapsTools/ES2N-Requisitos Funcionais v1.0 rev2609.xlsx
+++ b/CCapsTools/ES2N-Requisitos Funcionais v1.0 rev2609.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Aulas2024_2sem\AtividadesES2N\ERICKDEFARIAINACIO\CCapsTools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Github Denilce\ES2N\CCapsTools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F4BEDB-D2D7-4723-9F0D-31AE3D44321F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC6AC4D-CA90-4F5F-A99A-9B8DFCF81CEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="23452" windowHeight="12561" xr2:uid="{4ABF0B59-3EAA-4472-9014-1459B26A9A3B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4ABF0B59-3EAA-4472-9014-1459B26A9A3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -821,11 +821,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3837308E-2BE3-4051-9282-618B7392BE50}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.109375" style="10" customWidth="1"/>
     <col min="2" max="2" width="32.88671875" style="3" bestFit="1" customWidth="1"/>
@@ -836,7 +836,7 @@
     <col min="7" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -845,7 +845,7 @@
       <c r="D1" s="9"/>
       <c r="E1" s="12"/>
     </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
@@ -853,7 +853,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>2</v>
       </c>
@@ -873,7 +873,7 @@
       <c r="B6" s="6"/>
       <c r="C6" s="23"/>
     </row>
-    <row r="9" spans="1:6" s="5" customFormat="1" ht="60.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>3</v>
       </c>
@@ -890,7 +890,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="60.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>4</v>
       </c>
@@ -910,7 +910,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="45.4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>5</v>
       </c>
@@ -927,7 +927,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="45.4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>11</v>
       </c>
@@ -942,7 +942,7 @@
       </c>
       <c r="E12" s="25"/>
     </row>
-    <row r="13" spans="1:6" ht="60.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>12</v>
       </c>
@@ -957,7 +957,7 @@
       </c>
       <c r="E13" s="25"/>
     </row>
-    <row r="14" spans="1:6" ht="30.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>13</v>
       </c>
@@ -972,7 +972,7 @@
       </c>
       <c r="E14" s="25"/>
     </row>
-    <row r="15" spans="1:6" ht="60.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>14</v>
       </c>
@@ -989,7 +989,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="45.4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>15</v>
       </c>
@@ -1006,7 +1006,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="45.4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>16</v>
       </c>
@@ -1021,7 +1021,7 @@
       </c>
       <c r="E17" s="25"/>
     </row>
-    <row r="18" spans="1:5" ht="45.4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>21</v>
       </c>
@@ -1061,7 +1061,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="27" customFormat="1" ht="30.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="26">
         <v>12</v>
       </c>
@@ -1145,18 +1145,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1274,14 +1274,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9030A888-F94C-446A-AE50-538902A00351}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9386896A-91B6-4EC7-AC94-350129FCA8CC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1292,6 +1284,14 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9030A888-F94C-446A-AE50-538902A00351}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>